<commit_message>
Cleared extra prints, changed random limits
</commit_message>
<xml_diff>
--- a/GenerateApp/table/Table1.xlsx
+++ b/GenerateApp/table/Table1.xlsx
@@ -340,13 +340,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1">
         <v>1</v>
       </c>
@@ -371,31 +371,43 @@
       <c r="H1">
         <v>8</v>
       </c>
+      <c r="I1">
+        <v>9</v>
+      </c>
+      <c r="J1">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:10">
       <c r="A2">
-        <v>925</v>
+        <v>577</v>
       </c>
       <c r="B2">
-        <v>828</v>
+        <v>445</v>
       </c>
       <c r="C2">
-        <v>784</v>
+        <v>460</v>
       </c>
       <c r="D2">
-        <v>692</v>
+        <v>605</v>
       </c>
       <c r="E2">
-        <v>844</v>
+        <v>458</v>
       </c>
       <c r="F2">
-        <v>754</v>
+        <v>500</v>
       </c>
       <c r="G2">
-        <v>649</v>
+        <v>492</v>
       </c>
       <c r="H2">
-        <v>512</v>
+        <v>485</v>
+      </c>
+      <c r="I2">
+        <v>589</v>
+      </c>
+      <c r="J2">
+        <v>501</v>
       </c>
     </row>
   </sheetData>

</xml_diff>